<commit_message>
Modification du template généric pour ne faire défiler que les données
</commit_message>
<xml_diff>
--- a/apps/templates/xlsx/generic.xlsx
+++ b/apps/templates/xlsx/generic.xlsx
@@ -67,7 +67,7 @@
     <t xml:space="preserve">Business Keys</t>
   </si>
   <si>
-    <t xml:space="preserve">Commentaire</t>
+    <t xml:space="preserve">Comments</t>
   </si>
   <si>
     <t xml:space="preserve">Last Activity</t>
@@ -124,7 +124,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -132,13 +132,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -165,7 +158,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -174,11 +167,15 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -186,7 +183,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -209,47 +206,47 @@
   </sheetPr>
   <dimension ref="1:2"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="P1" activeCellId="0" sqref="P1"/>
-      <selection pane="bottomLeft" activeCell="C2" activeCellId="0" sqref="2:2"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="36.9540816326531"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.4183673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="14.8673469387755"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.9438775510204"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.1938775510204"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="37.5102040816326"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.3928571428571"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="17.6836734693878"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="1" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="12.9132653061225"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="30.984693877551"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="13.1938775510204"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="31" min="29" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="33" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="36.5816326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.7448979591837"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="37.1224489795918"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="17.4132653061224"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="1" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="31" min="29" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="33" style="1" width="10.6632653061225"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="49.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" s="5" customFormat="true" ht="49.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -277,59 +274,59 @@
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2" t="s">
+      <c r="K1" s="3"/>
+      <c r="L1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2" t="s">
+      <c r="M1" s="3"/>
+      <c r="N1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="2"/>
+      <c r="O1" s="3"/>
       <c r="P1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2" t="s">
+      <c r="R1" s="3"/>
+      <c r="S1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="T1" s="2"/>
+      <c r="T1" s="3"/>
       <c r="U1" s="2" t="s">
         <v>15</v>
       </c>
       <c r="V1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
-      <c r="AA1" s="3"/>
-      <c r="AB1" s="3"/>
-      <c r="AC1" s="3"/>
-      <c r="AD1" s="3"/>
-      <c r="AE1" s="3"/>
-      <c r="AF1" s="3"/>
-      <c r="ALY1" s="5"/>
-      <c r="ALZ1" s="5"/>
-      <c r="AMA1" s="5"/>
-      <c r="AMB1" s="5"/>
-      <c r="AMC1" s="5"/>
-      <c r="AMD1" s="5"/>
-      <c r="AME1" s="5"/>
-      <c r="AMF1" s="5"/>
-      <c r="AMG1" s="5"/>
-      <c r="AMH1" s="5"/>
-      <c r="AMI1" s="5"/>
-      <c r="AMJ1" s="5"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
+      <c r="AA1" s="4"/>
+      <c r="AB1" s="4"/>
+      <c r="AC1" s="4"/>
+      <c r="AD1" s="4"/>
+      <c r="AE1" s="4"/>
+      <c r="AF1" s="4"/>
+      <c r="ALY1" s="6"/>
+      <c r="ALZ1" s="6"/>
+      <c r="AMA1" s="6"/>
+      <c r="AMB1" s="6"/>
+      <c r="AMC1" s="6"/>
+      <c r="AMD1" s="6"/>
+      <c r="AME1" s="6"/>
+      <c r="AMF1" s="6"/>
+      <c r="AMG1" s="6"/>
+      <c r="AMH1" s="6"/>
+      <c r="AMI1" s="6"/>
+      <c r="AMJ1" s="6"/>
     </row>
-    <row r="2" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J2" s="2" t="s">
         <v>17</v>
       </c>
@@ -348,7 +345,7 @@
       <c r="O2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="P2" s="6" t="s">
         <v>18</v>
       </c>
       <c r="Q2" s="2" t="s">

</xml_diff>

<commit_message>
YNY_REPORTS: Fixing the timespents, added new column total time spent, calculating SKS timespents by (session_date_end - session_date_begin)
</commit_message>
<xml_diff>
--- a/apps/templates/xlsx/generic.xlsx
+++ b/apps/templates/xlsx/generic.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,63 +20,66 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
-  <si>
-    <t xml:space="preserve">Account</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contract</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prénom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acquired Level</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Recommended Level</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Training</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Start Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">End Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E-learning</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Skills Sessions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Catchup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Microlearning</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ESP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Business Keys</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Last Activity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Done</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Time</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>Contract</t>
+  </si>
+  <si>
+    <t>Nom</t>
+  </si>
+  <si>
+    <t>Prénom</t>
+  </si>
+  <si>
+    <t>Acquired Level</t>
+  </si>
+  <si>
+    <t>Recommended Level</t>
+  </si>
+  <si>
+    <t>Training</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>End Date</t>
+  </si>
+  <si>
+    <t>E-learning</t>
+  </si>
+  <si>
+    <t>Skills Sessions</t>
+  </si>
+  <si>
+    <t>Catchup</t>
+  </si>
+  <si>
+    <t>Microlearning</t>
+  </si>
+  <si>
+    <t>ESP</t>
+  </si>
+  <si>
+    <t>Business Keys</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Total Time</t>
+  </si>
+  <si>
+    <t>Last Activity</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Time</t>
   </si>
 </sst>
 </file>
@@ -84,7 +87,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -164,7 +167,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -206,44 +209,44 @@
   </sheetPr>
   <dimension ref="1:2"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="S1" activeCellId="0" sqref="S1"/>
+      <selection pane="bottomLeft" activeCell="AA15" activeCellId="0" sqref="AA15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="36.5816326530612"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.7448979591837"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="37.1224489795918"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="17.4132653061224"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="1" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="30.6428571428571"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="36.1785714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.4744897959184"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="36.719387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="17.1428571428571"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="1" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="23" min="22" style="1" width="12.8265306122449"/>
     <col collapsed="false" hidden="false" max="24" min="24" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="10.530612244898"/>
     <col collapsed="false" hidden="false" max="26" min="26" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="31" min="29" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="33" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="32" min="30" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="34" style="1" width="10.530612244898"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="49.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -303,7 +306,9 @@
       <c r="V1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="W1" s="4"/>
+      <c r="W1" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="X1" s="4"/>
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
@@ -313,7 +318,7 @@
       <c r="AD1" s="4"/>
       <c r="AE1" s="4"/>
       <c r="AF1" s="4"/>
-      <c r="ALY1" s="6"/>
+      <c r="AG1" s="4"/>
       <c r="ALZ1" s="6"/>
       <c r="AMA1" s="6"/>
       <c r="AMB1" s="6"/>
@@ -328,37 +333,37 @@
     </row>
     <row r="2" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J2" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="P2" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>